<commit_message>
Finaliza  migración de Controlador y DAO para ActividadTipo
</commit_message>
<xml_diff>
--- a/Avances/Avance Migracion Sipro.xlsx
+++ b/Avances/Avance Migracion Sipro.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\git\Sipro\Avances\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eescobedo.DC-DI01\Documents\Code\SiproDesaCSharp\Avances\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Controllers" sheetId="1" r:id="rId1"/>
@@ -1606,7 +1606,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1637,10 +1637,11 @@
     <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="16">
     <dxf>
@@ -1822,7 +1823,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2086,11 +2087,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86:D86"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
@@ -2170,7 +2171,7 @@
         <v>206</v>
       </c>
       <c r="D5" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="2"/>
     </row>
@@ -2184,7 +2185,7 @@
       <c r="C6" t="s">
         <v>212</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="16">
         <v>1</v>
       </c>
       <c r="E6" s="2"/>
@@ -3514,7 +3515,7 @@
       <c r="C97" s="4"/>
       <c r="D97">
         <f>COUNTIFS(D3:D94,100%)</f>
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
@@ -3534,7 +3535,7 @@
       <c r="C99" s="4"/>
       <c r="D99">
         <f>COUNTIFS(D3:D94,0%)</f>
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -3568,7 +3569,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3576,11 +3577,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.5703125" bestFit="1" customWidth="1"/>
@@ -4795,7 +4796,7 @@
       <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
@@ -5965,7 +5966,7 @@
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.28515625" bestFit="1" customWidth="1"/>
@@ -6938,7 +6939,7 @@
       <selection activeCell="B9" sqref="B9:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="60.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
@@ -7090,18 +7091,18 @@
       </c>
       <c r="D9" s="9">
         <f>Controllers!D97</f>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E9" s="11">
         <f t="shared" si="1"/>
-        <v>0.33695652173913043</v>
+        <v>0.34782608695652173</v>
       </c>
       <c r="F9" s="9">
         <v>40</v>
       </c>
       <c r="G9" s="12">
         <f t="shared" si="0"/>
-        <v>13.478260869565217</v>
+        <v>13.913043478260869</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -7185,7 +7186,7 @@
       </c>
       <c r="G13" s="12">
         <f>SUM(G4:G12)</f>
-        <v>81.674739090139823</v>
+        <v>82.109521698835465</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="33.75" x14ac:dyDescent="0.5">
@@ -7194,7 +7195,7 @@
       </c>
       <c r="C16" s="15">
         <f>G13/F13</f>
-        <v>0.38165765929971879</v>
+        <v>0.38368935373287599</v>
       </c>
       <c r="D16" s="15"/>
     </row>

</xml_diff>

<commit_message>
Finalizacion de actividad controller
</commit_message>
<xml_diff>
--- a/Avances/Avance Migracion Sipro.xlsx
+++ b/Avances/Avance Migracion Sipro.xlsx
@@ -1606,7 +1606,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1634,10 +1634,11 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2087,8 +2088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2141,7 +2142,7 @@
         <v>205</v>
       </c>
       <c r="D3" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="2"/>
     </row>
@@ -2185,7 +2186,7 @@
       <c r="C6" t="s">
         <v>212</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="15">
         <v>1</v>
       </c>
       <c r="E6" s="2"/>
@@ -3515,7 +3516,7 @@
       <c r="C97" s="4"/>
       <c r="D97">
         <f>COUNTIFS(D3:D94,100%)</f>
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
@@ -3535,7 +3536,7 @@
       <c r="C99" s="4"/>
       <c r="D99">
         <f>COUNTIFS(D3:D94,0%)</f>
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -3575,10 +3576,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C110"/>
+  <dimension ref="A1:F110"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3586,9 +3587,10 @@
     <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>117</v>
       </c>
@@ -3599,7 +3601,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -3607,10 +3609,17 @@
         <v>31</v>
       </c>
       <c r="C2" s="3">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.31</v>
+      </c>
+      <c r="E2">
+        <f>10/32</f>
+        <v>0.3125</v>
+      </c>
+      <c r="F2" s="17">
+        <v>43350</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -3621,7 +3630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -3629,10 +3638,10 @@
         <v>33</v>
       </c>
       <c r="C4" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -3640,10 +3649,10 @@
         <v>34</v>
       </c>
       <c r="C5" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -3654,7 +3663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -3665,7 +3674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -3676,7 +3685,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -3687,7 +3696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -3698,7 +3707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -3709,7 +3718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -3720,7 +3729,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -3731,7 +3740,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -3742,7 +3751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -3753,7 +3762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -4749,7 +4758,7 @@
       </c>
       <c r="C108">
         <f>COUNTIFS(C2:C105,100%)</f>
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -4767,7 +4776,7 @@
       </c>
       <c r="C110">
         <f>COUNTIFS(C2:C105,0%)</f>
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -7067,18 +7076,18 @@
       </c>
       <c r="D8" s="9">
         <f>Daos!C108</f>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E8" s="11">
         <f t="shared" si="1"/>
-        <v>0.42307692307692307</v>
+        <v>0.44230769230769229</v>
       </c>
       <c r="F8" s="9">
         <v>20</v>
       </c>
       <c r="G8" s="12">
         <f t="shared" si="0"/>
-        <v>8.4615384615384617</v>
+        <v>8.8461538461538467</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -7091,18 +7100,18 @@
       </c>
       <c r="D9" s="9">
         <f>Controllers!D97</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E9" s="11">
         <f t="shared" si="1"/>
-        <v>0.34782608695652173</v>
+        <v>0.35869565217391303</v>
       </c>
       <c r="F9" s="9">
         <v>40</v>
       </c>
       <c r="G9" s="12">
         <f t="shared" si="0"/>
-        <v>13.913043478260869</v>
+        <v>14.347826086956522</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -7186,18 +7195,18 @@
       </c>
       <c r="G13" s="12">
         <f>SUM(G4:G12)</f>
-        <v>82.109521698835465</v>
+        <v>82.928919692146508</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="33.75" x14ac:dyDescent="0.5">
       <c r="B16" s="14" t="s">
         <v>313</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="16">
         <f>G13/F13</f>
-        <v>0.38368935373287599</v>
-      </c>
-      <c r="D16" s="15"/>
+        <v>0.38751831631844164</v>
+      </c>
+      <c r="D16" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Modificacion de avances en excel
</commit_message>
<xml_diff>
--- a/Avances/Avance Migracion Sipro.xlsx
+++ b/Avances/Avance Migracion Sipro.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Controllers" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="504">
   <si>
     <t>Controllers</t>
   </si>
@@ -2113,8 +2113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2167,7 +2167,7 @@
         <v>205</v>
       </c>
       <c r="D3" s="3">
-        <v>0.15</v>
+        <v>1</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>499</v>
@@ -2184,7 +2184,7 @@
         <v>211</v>
       </c>
       <c r="D4" s="3">
-        <v>0.88</v>
+        <v>1</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>500</v>
@@ -2312,7 +2312,7 @@
         <v>214</v>
       </c>
       <c r="D12" s="3">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>501</v>
@@ -3356,7 +3356,9 @@
       <c r="D78" s="3">
         <v>0</v>
       </c>
-      <c r="E78" s="15"/>
+      <c r="E78" s="16" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
@@ -3371,7 +3373,9 @@
       <c r="D79" s="3">
         <v>0</v>
       </c>
-      <c r="E79" s="15"/>
+      <c r="E79" s="16" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
@@ -3386,7 +3390,9 @@
       <c r="D80" s="3">
         <v>0</v>
       </c>
-      <c r="E80" s="15"/>
+      <c r="E80" s="16" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
@@ -3480,10 +3486,10 @@
         <v>287</v>
       </c>
       <c r="D86" s="3">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="E86" s="16" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -3623,7 +3629,7 @@
       <c r="C97" s="18"/>
       <c r="D97">
         <f>COUNTIFS(D3:D94,100%)</f>
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
@@ -3633,7 +3639,7 @@
       <c r="C98" s="18"/>
       <c r="D98">
         <f>COUNTIFS(D3:D94,"&gt;"&amp; 0%,D3:D94,"&lt;" &amp; 100%)</f>
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.25">
@@ -3691,7 +3697,7 @@
   <dimension ref="A1:D110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3724,7 +3730,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="3">
-        <v>0.15</v>
+        <v>0.08</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>499</v>
@@ -3738,7 +3744,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="3">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="17" t="s">
         <v>500</v>
@@ -3752,10 +3758,10 @@
         <v>33</v>
       </c>
       <c r="C4" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3816,10 +3822,10 @@
         <v>37</v>
       </c>
       <c r="C9" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3846,6 +3852,9 @@
       <c r="C11" s="3">
         <v>1</v>
       </c>
+      <c r="D11" s="17" t="s">
+        <v>501</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
@@ -4758,6 +4767,9 @@
       <c r="C83" s="1">
         <v>0</v>
       </c>
+      <c r="D83" s="17" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
@@ -4769,6 +4781,9 @@
       <c r="C84" s="1">
         <v>0</v>
       </c>
+      <c r="D84" s="17" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
@@ -4780,6 +4795,9 @@
       <c r="C85" s="1">
         <v>0</v>
       </c>
+      <c r="D85" s="17" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
@@ -4791,6 +4809,9 @@
       <c r="C86" s="1">
         <v>0</v>
       </c>
+      <c r="D86" s="17" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
@@ -5052,7 +5073,7 @@
       </c>
       <c r="C108">
         <f>COUNTIFS(C2:C105,100%)</f>
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -5061,7 +5082,7 @@
       </c>
       <c r="C109">
         <f>COUNTIFS(C2:C105,"&gt;"&amp; 0%,C2:C105,"&lt;" &amp; 100%)</f>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -5070,7 +5091,7 @@
       </c>
       <c r="C110">
         <f>COUNTIFS(C2:C105,0%)</f>
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -5095,9 +5116,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B103" sqref="B103:B105"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6570,7 +6589,7 @@
   <dimension ref="A1:D88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B86" sqref="B86:B88"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6617,10 +6636,10 @@
         <v>418</v>
       </c>
       <c r="C3" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -6645,7 +6664,10 @@
         <v>420</v>
       </c>
       <c r="C5" s="3">
-        <v>0</v>
+        <v>0.45</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -7399,6 +7421,9 @@
       <c r="C69" s="3">
         <v>0</v>
       </c>
+      <c r="D69" s="17" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
@@ -7410,6 +7435,9 @@
       <c r="C70" s="3">
         <v>0</v>
       </c>
+      <c r="D70" s="17" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
@@ -7421,6 +7449,9 @@
       <c r="C71" s="3">
         <v>0</v>
       </c>
+      <c r="D71" s="17" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
@@ -7578,7 +7609,7 @@
       </c>
       <c r="C86">
         <f>COUNTIFS(C2:C83,100%)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -7587,7 +7618,7 @@
       </c>
       <c r="C87">
         <f>COUNTIFS(C2:C83,"&gt;"&amp; 0%,C2:C83,"&lt;" &amp; 100%)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -7596,7 +7627,7 @@
       </c>
       <c r="C88">
         <f>COUNTIFS(C2:C83,0%)</f>
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -7621,7 +7652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G16"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -7753,18 +7784,18 @@
       </c>
       <c r="D8" s="9">
         <f>Daos!C108</f>
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E8" s="11">
         <f t="shared" si="1"/>
-        <v>0.45192307692307693</v>
+        <v>0.48076923076923078</v>
       </c>
       <c r="F8" s="9">
         <v>20</v>
       </c>
       <c r="G8" s="12">
         <f t="shared" si="0"/>
-        <v>9.0384615384615383</v>
+        <v>9.615384615384615</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -7777,18 +7808,18 @@
       </c>
       <c r="D9" s="9">
         <f>Controllers!D97</f>
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E9" s="11">
         <f t="shared" si="1"/>
-        <v>0.34782608695652173</v>
+        <v>0.39130434782608697</v>
       </c>
       <c r="F9" s="9">
         <v>40</v>
       </c>
       <c r="G9" s="12">
         <f t="shared" si="0"/>
-        <v>13.913043478260869</v>
+        <v>15.652173913043478</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -7821,18 +7852,18 @@
         <v>83</v>
       </c>
       <c r="D11" s="9">
-        <v>23</v>
+        <v>23.85</v>
       </c>
       <c r="E11" s="11">
         <f t="shared" si="1"/>
-        <v>0.27710843373493976</v>
+        <v>0.28734939759036149</v>
       </c>
       <c r="F11" s="9">
         <v>120</v>
       </c>
       <c r="G11" s="12">
         <f t="shared" si="0"/>
-        <v>33.253012048192772</v>
+        <v>34.481927710843379</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
@@ -7872,7 +7903,7 @@
       </c>
       <c r="G13" s="12">
         <f>SUM(G4:G12)</f>
-        <v>90.20451706491518</v>
+        <v>93.749486239271477</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="33.75" x14ac:dyDescent="0.5">
@@ -7881,7 +7912,7 @@
       </c>
       <c r="C16" s="19">
         <f>G13/F13</f>
-        <v>0.42151643488278123</v>
+        <v>0.43808171139846486</v>
       </c>
       <c r="D16" s="19"/>
     </row>

</xml_diff>

<commit_message>
Se agrega categoria de adquisición
</commit_message>
<xml_diff>
--- a/Avances/Avance Migracion Sipro.xlsx
+++ b/Avances/Avance Migracion Sipro.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="504">
   <si>
     <t>Controllers</t>
   </si>
@@ -6589,7 +6589,7 @@
   <dimension ref="A1:D88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6678,7 +6678,10 @@
         <v>421</v>
       </c>
       <c r="C6" s="3">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -7609,7 +7612,7 @@
       </c>
       <c r="C86">
         <f>COUNTIFS(C2:C83,100%)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -7627,7 +7630,7 @@
       </c>
       <c r="C88">
         <f>COUNTIFS(C2:C83,0%)</f>
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -7852,18 +7855,18 @@
         <v>83</v>
       </c>
       <c r="D11" s="9">
-        <v>23.85</v>
+        <v>24.85</v>
       </c>
       <c r="E11" s="11">
         <f t="shared" si="1"/>
-        <v>0.28734939759036149</v>
+        <v>0.29939759036144581</v>
       </c>
       <c r="F11" s="9">
         <v>120</v>
       </c>
       <c r="G11" s="12">
         <f t="shared" si="0"/>
-        <v>34.481927710843379</v>
+        <v>35.927710843373497</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
@@ -7903,7 +7906,7 @@
       </c>
       <c r="G13" s="12">
         <f>SUM(G4:G12)</f>
-        <v>93.749486239271477</v>
+        <v>95.195269371801587</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="33.75" x14ac:dyDescent="0.5">
@@ -7912,7 +7915,7 @@
       </c>
       <c r="C16" s="19">
         <f>G13/F13</f>
-        <v>0.43808171139846486</v>
+        <v>0.44483770734486722</v>
       </c>
       <c r="D16" s="19"/>
     </row>

</xml_diff>

<commit_message>
Se agregan cambios de tipo de adquisición
</commit_message>
<xml_diff>
--- a/Avances/Avance Migracion Sipro.xlsx
+++ b/Avances/Avance Migracion Sipro.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Controllers" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="504">
   <si>
     <t>Controllers</t>
   </si>
@@ -2113,8 +2113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3552,9 +3552,11 @@
         <v>291</v>
       </c>
       <c r="D90" s="3">
-        <v>0</v>
-      </c>
-      <c r="E90" s="15"/>
+        <v>1</v>
+      </c>
+      <c r="E90" s="16" t="s">
+        <v>501</v>
+      </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
@@ -3629,7 +3631,7 @@
       <c r="C97" s="18"/>
       <c r="D97">
         <f>COUNTIFS(D3:D94,100%)</f>
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
@@ -3649,7 +3651,7 @@
       <c r="C99" s="18"/>
       <c r="D99">
         <f>COUNTIFS(D3:D94,0%)</f>
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -3696,8 +3698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D110"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6588,8 +6590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7560,6 +7562,9 @@
       </c>
       <c r="C79" s="3">
         <v>0</v>
+      </c>
+      <c r="D79" s="17" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -7655,7 +7660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -7811,18 +7816,18 @@
       </c>
       <c r="D9" s="9">
         <f>Controllers!D97</f>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E9" s="11">
         <f t="shared" si="1"/>
-        <v>0.39130434782608697</v>
+        <v>0.40217391304347827</v>
       </c>
       <c r="F9" s="9">
         <v>40</v>
       </c>
       <c r="G9" s="12">
         <f t="shared" si="0"/>
-        <v>15.652173913043478</v>
+        <v>16.086956521739133</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -7906,7 +7911,7 @@
       </c>
       <c r="G13" s="12">
         <f>SUM(G4:G12)</f>
-        <v>95.195269371801587</v>
+        <v>95.630051980497242</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="33.75" x14ac:dyDescent="0.5">
@@ -7915,7 +7920,7 @@
       </c>
       <c r="C16" s="19">
         <f>G13/F13</f>
-        <v>0.44483770734486722</v>
+        <v>0.44686940177802448</v>
       </c>
       <c r="D16" s="19"/>
     </row>

</xml_diff>

<commit_message>
Cambios realizados en Actividad
</commit_message>
<xml_diff>
--- a/Avances/Avance Migracion Sipro.xlsx
+++ b/Avances/Avance Migracion Sipro.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="504">
   <si>
     <t>Controllers</t>
   </si>
@@ -2113,8 +2113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2790,9 +2790,11 @@
         <v>243</v>
       </c>
       <c r="D42" s="3">
-        <v>0</v>
-      </c>
-      <c r="E42" s="15"/>
+        <v>0.6</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>501</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
@@ -2880,9 +2882,11 @@
         <v>249</v>
       </c>
       <c r="D48" s="3">
-        <v>0</v>
-      </c>
-      <c r="E48" s="15"/>
+        <v>1</v>
+      </c>
+      <c r="E48" s="16" t="s">
+        <v>501</v>
+      </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
@@ -3631,7 +3635,7 @@
       <c r="C97" s="18"/>
       <c r="D97">
         <f>COUNTIFS(D3:D94,100%)</f>
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
@@ -3641,7 +3645,7 @@
       <c r="C98" s="18"/>
       <c r="D98">
         <f>COUNTIFS(D3:D94,"&gt;"&amp; 0%,D3:D94,"&lt;" &amp; 100%)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.25">
@@ -3651,7 +3655,7 @@
       <c r="C99" s="18"/>
       <c r="D99">
         <f>COUNTIFS(D3:D94,0%)</f>
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -3699,7 +3703,7 @@
   <dimension ref="A1:D110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3813,7 +3817,10 @@
         <v>36</v>
       </c>
       <c r="C8" s="3">
-        <v>0.05</v>
+        <v>1</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -5075,7 +5082,7 @@
       </c>
       <c r="C108">
         <f>COUNTIFS(C2:C105,100%)</f>
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -5084,7 +5091,7 @@
       </c>
       <c r="C109">
         <f>COUNTIFS(C2:C105,"&gt;"&amp; 0%,C2:C105,"&lt;" &amp; 100%)</f>
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -7792,18 +7799,18 @@
       </c>
       <c r="D8" s="9">
         <f>Daos!C108</f>
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E8" s="11">
         <f t="shared" si="1"/>
-        <v>0.49038461538461536</v>
+        <v>0.5</v>
       </c>
       <c r="F8" s="9">
         <v>20</v>
       </c>
       <c r="G8" s="12">
         <f t="shared" si="0"/>
-        <v>9.8076923076923066</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -7816,18 +7823,18 @@
       </c>
       <c r="D9" s="9">
         <f>Controllers!D97</f>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E9" s="11">
         <f t="shared" si="1"/>
-        <v>0.40217391304347827</v>
+        <v>0.41304347826086957</v>
       </c>
       <c r="F9" s="9">
         <v>40</v>
       </c>
       <c r="G9" s="12">
         <f t="shared" si="0"/>
-        <v>16.086956521739133</v>
+        <v>16.521739130434781</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -7911,7 +7918,7 @@
       </c>
       <c r="G13" s="12">
         <f>SUM(G4:G12)</f>
-        <v>98.930793407744687</v>
+        <v>99.557883708748037</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="33.75" x14ac:dyDescent="0.5">
@@ -7920,7 +7927,7 @@
       </c>
       <c r="C16" s="19">
         <f>G13/F13</f>
-        <v>0.46229342713899385</v>
+        <v>0.46522375564835533</v>
       </c>
       <c r="D16" s="19"/>
     </row>

</xml_diff>